<commit_message>
Update 19.04. und Datenvollständigkeit
</commit_message>
<xml_diff>
--- a/Mobility_VerkehrsmessstellenKantonZH_Datenvollständigkeit.xlsx
+++ b/Mobility_VerkehrsmessstellenKantonZH_Datenvollständigkeit.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>Messstelle</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>8.-14.4.2020 keine Daten</t>
+  </si>
+  <si>
+    <t>ab 15.04.2020 keine Daten; grössere Bautätigkeiten</t>
   </si>
 </sst>
 </file>
@@ -509,7 +512,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,6 +580,9 @@
       </c>
       <c r="B6" t="s">
         <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update Woche 1, Dez. 2020
</commit_message>
<xml_diff>
--- a/Mobility_VerkehrsmessstellenKantonZH_Datenvollständigkeit.xlsx
+++ b/Mobility_VerkehrsmessstellenKantonZH_Datenvollständigkeit.xlsx
@@ -132,9 +132,6 @@
     <t>Ostermontag</t>
   </si>
   <si>
-    <t>ab 15.04.2020 keine Daten; grössere Bautätigkeiten</t>
-  </si>
-  <si>
     <t>Tag der Arbeit</t>
   </si>
   <si>
@@ -161,6 +158,9 @@
     <t>8.-14.4.2020, 
 27.04. - 4.05.2020; technische Störung
 06.05.-11.06.2020; technische Störung</t>
+  </si>
+  <si>
+    <t>15.04..30.11.2020 keine Daten; grössere Bautätigkeiten</t>
   </si>
 </sst>
 </file>
@@ -550,7 +550,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,7 +584,7 @@
         <v>2020</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -595,7 +595,7 @@
         <v>23</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -620,7 +620,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3690</v>
       </c>
@@ -628,10 +628,10 @@
         <v>4</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>109</v>
       </c>
@@ -639,7 +639,7 @@
         <v>5</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -651,7 +651,7 @@
       </c>
       <c r="D8" s="10"/>
     </row>
-    <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5191</v>
       </c>
@@ -659,7 +659,7 @@
         <v>7</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -723,10 +723,10 @@
         <v>3</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F15" s="13"/>
       <c r="G15" s="13"/>
@@ -744,7 +744,7 @@
         <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -889,7 +889,7 @@
         <v>43952</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 2. Woche Dezember 2020
</commit_message>
<xml_diff>
--- a/Mobility_VerkehrsmessstellenKantonZH_Datenvollständigkeit.xlsx
+++ b/Mobility_VerkehrsmessstellenKantonZH_Datenvollständigkeit.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7056"/>
   </bookViews>
   <sheets>
     <sheet name="Techn.Unterbrüche" sheetId="1" r:id="rId1"/>
@@ -141,10 +141,6 @@
     <t>ab 22.05.2020 keine Daten; technische Störung</t>
   </si>
   <si>
-    <t>06.05.-11.06.2020 keine Daten aufgrund techn. Defekt.
-Daten ab 27.04.: Aufgrund technischer Störung kann es zu einer fehlerhaften Klassifizierung gekommen sein. Total stimmt, Anz. Motorrad ggf. zu viele ausgewiesen.</t>
-  </si>
-  <si>
     <t>21.05.-3.6.2020 keine Daten; technische Störung</t>
   </si>
   <si>
@@ -161,6 +157,9 @@
   </si>
   <si>
     <t>15.04..30.11.2020 keine Daten; grössere Bautätigkeiten</t>
+  </si>
+  <si>
+    <t>Daten ab 27.04.: Aufgrund technischer Störung kann es zu einer fehlerhaften Klassifizierung gekommen sein. Total stimmt, Anz. Motorrad ggf. zu viele ausgewiesen.</t>
   </si>
 </sst>
 </file>
@@ -550,18 +549,18 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="57.7109375" customWidth="1"/>
-    <col min="5" max="5" width="50.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.6640625" customWidth="1"/>
+    <col min="5" max="5" width="50.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -570,7 +569,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -587,7 +586,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1887</v>
       </c>
@@ -595,10 +594,10 @@
         <v>23</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>110</v>
       </c>
@@ -609,7 +608,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5186</v>
       </c>
@@ -620,7 +619,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3690</v>
       </c>
@@ -628,10 +627,10 @@
         <v>4</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>109</v>
       </c>
@@ -642,7 +641,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1288</v>
       </c>
@@ -651,7 +650,7 @@
       </c>
       <c r="D8" s="10"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>5191</v>
       </c>
@@ -659,10 +658,10 @@
         <v>7</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2085</v>
       </c>
@@ -676,7 +675,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>3687</v>
       </c>
@@ -688,7 +687,7 @@
       </c>
       <c r="D11" s="10"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>609</v>
       </c>
@@ -697,7 +696,7 @@
       </c>
       <c r="D12" s="10"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>208</v>
       </c>
@@ -706,7 +705,7 @@
       </c>
       <c r="D13" s="10"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2287</v>
       </c>
@@ -715,7 +714,7 @@
       </c>
       <c r="D14" s="10"/>
     </row>
-    <row r="15" spans="1:12" s="11" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" s="11" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11">
         <v>587</v>
       </c>
@@ -723,10 +722,10 @@
         <v>3</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="F15" s="13"/>
       <c r="G15" s="13"/>
@@ -736,7 +735,7 @@
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1109</v>
       </c>
@@ -744,10 +743,10 @@
         <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>4790</v>
       </c>
@@ -755,7 +754,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>17</v>
       </c>
@@ -763,7 +762,7 @@
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>316</v>
       </c>
@@ -771,7 +770,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>716</v>
       </c>
@@ -779,7 +778,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1018</v>
       </c>
@@ -787,7 +786,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2019</v>
       </c>
@@ -814,13 +813,13 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>26</v>
       </c>
@@ -828,7 +827,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>43831</v>
       </c>
@@ -836,7 +835,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>43832</v>
       </c>
@@ -844,7 +843,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>43836</v>
       </c>
@@ -852,7 +851,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>43887</v>
       </c>
@@ -860,7 +859,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>43931</v>
       </c>
@@ -868,7 +867,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>43933</v>
       </c>
@@ -876,7 +875,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>43934</v>
       </c>
@@ -884,7 +883,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>43952</v>
       </c>

</xml_diff>